<commit_message>
Ya están guardados los que funcionan
</commit_message>
<xml_diff>
--- a/EleccionesCAM2023.xlsx
+++ b/EleccionesCAM2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\dipus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D936C947-847A-4CB4-AF42-E80A49B35EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BE3CF6-E4D2-4A23-9F87-D5B70423C4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{AC4A673A-371C-4FF6-B49E-25028415119F}"/>
   </bookViews>
@@ -165,9 +165,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +207,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -229,20 +236,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -558,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89A283A-C569-4E7A-AF15-C5356B3E6CF4}">
-  <dimension ref="A1:AQ7"/>
+  <dimension ref="A1:AQ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AR2" sqref="AR2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,165 +783,165 @@
       <c r="Q2" s="3">
         <v>135</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="7">
         <v>1599186</v>
       </c>
       <c r="S2" s="3">
         <v>70</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2" s="7">
         <v>7219</v>
       </c>
       <c r="U2" s="3">
         <v>0</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="7">
         <v>614296</v>
       </c>
       <c r="W2" s="3">
         <v>27</v>
       </c>
-      <c r="X2" s="3">
+      <c r="X2" s="7">
         <v>2544</v>
       </c>
       <c r="Y2" s="3">
         <v>0</v>
       </c>
-      <c r="Z2" s="3">
+      <c r="Z2" s="7">
         <v>2404</v>
       </c>
       <c r="AA2" s="3">
         <v>0</v>
       </c>
-      <c r="AB2" s="3">
+      <c r="AB2" s="7">
         <v>4148</v>
       </c>
       <c r="AC2" s="3">
         <v>0</v>
       </c>
-      <c r="AD2" s="3">
+      <c r="AD2" s="7">
         <v>620631</v>
       </c>
       <c r="AE2" s="3">
         <v>27</v>
       </c>
-      <c r="AF2" s="3">
+      <c r="AF2" s="7">
         <v>52925</v>
       </c>
       <c r="AG2" s="3">
         <v>0</v>
       </c>
-      <c r="AH2" s="3">
+      <c r="AH2" s="7">
         <v>23451</v>
       </c>
       <c r="AI2" s="3">
         <v>0</v>
       </c>
-      <c r="AJ2" s="3">
+      <c r="AJ2" s="7">
         <v>2779</v>
       </c>
       <c r="AK2" s="3">
         <v>0</v>
       </c>
-      <c r="AL2" s="3">
+      <c r="AL2" s="7">
         <v>248379</v>
       </c>
       <c r="AM2" s="3">
         <v>11</v>
       </c>
-      <c r="AN2" s="3">
+      <c r="AN2" s="7">
         <v>161032</v>
       </c>
       <c r="AO2" s="3">
         <v>0</v>
       </c>
-      <c r="AP2" s="3">
+      <c r="AP2" s="7">
         <v>5376</v>
       </c>
       <c r="AQ2" s="3">
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="4"/>
+      <c r="AP4" s="4"/>
+    </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4"/>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="4"/>
-      <c r="AK5" s="4"/>
-      <c r="AL5" s="4"/>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="4"/>
-      <c r="AO5" s="4"/>
-      <c r="AP5" s="4"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="5"/>
-      <c r="AG6" s="5"/>
-      <c r="AH6" s="5"/>
-      <c r="AI6" s="5"/>
-      <c r="AJ6" s="5"/>
-      <c r="AK6" s="5"/>
-      <c r="AL6" s="5"/>
-      <c r="AM6" s="5"/>
-      <c r="AN6" s="5"/>
-      <c r="AO6" s="5"/>
-      <c r="AP6" s="5"/>
-    </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-      <c r="AE7" s="2"/>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
-      <c r="AI7" s="2"/>
-      <c r="AJ7" s="2"/>
-      <c r="AK7" s="2"/>
-      <c r="AL7" s="2"/>
-      <c r="AM7" s="2"/>
-      <c r="AN7" s="2"/>
-      <c r="AO7" s="2"/>
-      <c r="AP7" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>